<commit_message>
new rtl and new asserts
</commit_message>
<xml_diff>
--- a/Docs/DV Plan_FIFO_Memory.xlsx
+++ b/Docs/DV Plan_FIFO_Memory.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27729"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25623081-3C99-400E-90E5-3AA936FBD4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEB28821-672E-4F89-846A-85634FF464E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="89">
   <si>
     <t>Category</t>
   </si>
@@ -96,14 +96,215 @@
     <t>Implemented</t>
   </si>
   <si>
+    <t>Full_notWriteEn</t>
+  </si>
+  <si>
+    <t>joanna</t>
+  </si>
+  <si>
+    <t>The property assures that if FIFO is full then write enable signal must not be active.</t>
+  </si>
+  <si>
+    <t>Empty_notReadEn</t>
+  </si>
+  <si>
+    <t>The property assures that if FIFO is empty then read enable signal must not be active.</t>
+  </si>
+  <si>
+    <t>wrPtr_increm_writeEn_ON</t>
+  </si>
+  <si>
+    <t>The property assures that write pointer increments when a write operation happen</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>rdPtr_increm_rdEn_ON</t>
+  </si>
+  <si>
+    <t>The property assures that read pointer increments when a read operation happen.</t>
+  </si>
+  <si>
+    <t>wrPtrNext_increm_writeEn_ON</t>
+  </si>
+  <si>
+    <t>The property assures that wrPtrNext increments when a write operation happen</t>
+  </si>
+  <si>
+    <t>rdPtrNext_increm_rdEn_ON</t>
+  </si>
+  <si>
+    <t>The property assures that rdPtrNext  increments when a read operation happen.</t>
+  </si>
+  <si>
+    <t>wrEn_OFF_wrPtr_stable</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>The property assures that wrPtr is stable if a write doesn't occur.</t>
+  </si>
+  <si>
+    <t>rdEn_OFF_rdPtr_stable</t>
+  </si>
+  <si>
+    <t>The property assures that rdPtr is stable if a read doesn't occur.</t>
+  </si>
+  <si>
+    <t>rst_rdPtr_wrPtr_zero</t>
+  </si>
+  <si>
+    <t>after reset the read and write pointers must have the same value and be 0</t>
+  </si>
+  <si>
+    <t>rst_readEnOff_until_writeEnOn</t>
+  </si>
+  <si>
+    <t>after reset is active read enable is off until a write operation happens.</t>
+  </si>
+  <si>
+    <t>never_full_and_empty</t>
+  </si>
+  <si>
+    <t>ana</t>
+  </si>
+  <si>
+    <t>The full and empty flags can never be active at the same time.</t>
+  </si>
+  <si>
+    <t>wrPtrNext_maxvalue_reset0</t>
+  </si>
+  <si>
+    <t>when wrPtrNext reaches max value wraps around to 0</t>
+  </si>
+  <si>
+    <t>rdPtrNext_maxvalue_reset0</t>
+  </si>
+  <si>
+    <t>when rdPtrNext reaches max value wraps around to 0</t>
+  </si>
+  <si>
+    <t>wrPtr_maxvalue_reset0</t>
+  </si>
+  <si>
+    <t>when wrPtr reaches max value wraps around to 0</t>
+  </si>
+  <si>
+    <t>rdPtr_maxvalue_reset0</t>
+  </si>
+  <si>
+    <t>when rdPtr reaches max value wraps around to 0</t>
+  </si>
+  <si>
+    <t>empty_ON_whenreset</t>
+  </si>
+  <si>
+    <t>empty signal active when reset</t>
+  </si>
+  <si>
+    <t>full_OFF_whenreset</t>
+  </si>
+  <si>
+    <t>full signal off when reset</t>
+  </si>
+  <si>
+    <t>write_correctly</t>
+  </si>
+  <si>
+    <t>This property verifies that the writeData was writen correctly when the writeEn is activated</t>
+  </si>
+  <si>
+    <t>read_correctly</t>
+  </si>
+  <si>
+    <t>This property verifies that the readData was read correctly when readEn is activated</t>
+  </si>
+  <si>
+    <t>writeEnOff_rstOn</t>
+  </si>
+  <si>
+    <t>Assume write enable is not active when rst = 1</t>
+  </si>
+  <si>
+    <t>readEnOff_rstOn</t>
+  </si>
+  <si>
+    <t>Assume read enable is not active when rst = 1</t>
+  </si>
+  <si>
+    <t>FIFO_full</t>
+  </si>
+  <si>
+    <t>Cover that the FIFO becomes full</t>
+  </si>
+  <si>
+    <t>FIFO_empty</t>
+  </si>
+  <si>
+    <t>Cover that the FIFO becomes empty</t>
+  </si>
+  <si>
+    <t>FIFO_notFull</t>
+  </si>
+  <si>
+    <t>Cover that the write enable signal is asserted when the FIFO is not full</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  FIFO_notEmpty</t>
+  </si>
+  <si>
+    <t>Cover that the read enable signal is asserted when the FIFO is not empty</t>
+  </si>
+  <si>
+    <t>write_all_address</t>
+  </si>
+  <si>
+    <t>agregar cover  y logica auxiliar  para verficar si se escribio en todas las direcciones de memoria</t>
+  </si>
+  <si>
+    <t>read_all_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agregar cover si todos los posibles valores se escribieron en la memoria </t>
+  </si>
+  <si>
+    <t>como cover:que pasaria si el wrtieEn se levanta y la fifo esta llena</t>
+  </si>
+  <si>
+    <t>como cover  y su contraparte cuando la fifo este vacia</t>
+  </si>
+  <si>
+    <t>como cover: hacer una lectura y escritura a la vez</t>
+  </si>
+  <si>
+    <t>write_and_read_mem_full</t>
+  </si>
+  <si>
+    <t>Read and write at the same time while the memory is full.</t>
+  </si>
+  <si>
+    <t>write_and_read_mem_empty</t>
+  </si>
+  <si>
+    <t>Read and write at the same time while the memory is empty.</t>
+  </si>
+  <si>
+    <t>si el write pointer es menor al el read pointer, para el siguiente flanco el write pointer puede mayor que el read pointer? y su contraparte y justificar si se esta verificando con el plan ()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cambiar los parametros de la memoria, y ver si resultan en inderminados o contraejemplos, el bound y generar una grafica y un reporte sobre esos resultados, probar escenerios especificos en formal, hacer constraints 			</t>
+  </si>
+  <si>
+    <t>justificar como con el dv plan estamos verificando que el primer dato que entra es el primer dato que va a salir, el orden es el correcto?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,8 +374,26 @@
       <name val="Google Sans"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="6"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,8 +424,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -394,11 +637,115 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -412,9 +759,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -466,9 +810,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
@@ -485,6 +826,84 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -821,19 +1240,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J12"/>
+  <dimension ref="B2:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
+    <col min="7" max="7" width="47.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" customWidth="1"/>
@@ -842,191 +1262,889 @@
   <sheetData>
     <row r="2" spans="2:10" ht="30">
       <c r="B2" s="1"/>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="29"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="2:10">
       <c r="B3" s="4"/>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="2:10" ht="23.25">
       <c r="B4" s="4"/>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="D4" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="2:10" ht="23.25">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="2:10">
       <c r="B5" s="4"/>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="2:10">
-      <c r="B6" s="13"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="14" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="6"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="13"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="6"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="11"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="2:10" ht="36">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="17"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12" t="s">
+    <row r="10" spans="2:10" ht="23.25">
+      <c r="B10" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="17"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="17"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
+      <c r="C10" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="2:10" ht="23.25">
+      <c r="B11" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="37"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="2:10" ht="24">
+      <c r="B12" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="2:10" ht="23.25">
+      <c r="B13" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="2:10" ht="23.25">
+      <c r="B14" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="2:10" ht="23.25">
+      <c r="B15" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="2:10" ht="23.25">
+      <c r="B16" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="2:10" ht="23.25">
+      <c r="B17" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="2:10" ht="29.25">
+      <c r="B18" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="43"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+    </row>
+    <row r="19" spans="2:10" ht="29.25">
+      <c r="B19" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="43"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+    </row>
+    <row r="20" spans="2:10" ht="29.25">
+      <c r="B20" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="43"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="43"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" s="43"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="43"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="43"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="43"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="43"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="2:10" ht="29.25">
+      <c r="B27" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="43"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" spans="2:10" ht="24">
+      <c r="B28" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" s="43"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="37"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+    </row>
+    <row r="33" spans="2:10" ht="24">
+      <c r="B33" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+    </row>
+    <row r="34" spans="2:10" ht="24">
+      <c r="B34" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H34" s="49"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="55"/>
+    </row>
+    <row r="35" spans="2:10" ht="29.25">
+      <c r="B35" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="H35" s="47"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+    </row>
+    <row r="36" spans="2:10" ht="29.25">
+      <c r="B36" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
+    </row>
+    <row r="37" spans="2:10" ht="23.25">
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="48"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="48"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+    </row>
+    <row r="40" spans="2:10" ht="24" customHeight="1">
+      <c r="B40" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
+    </row>
+    <row r="41" spans="2:10" ht="24">
+      <c r="B41" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="G45" s="37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="G46" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="G47" s="10" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F12" xr:uid="{860860E9-2318-4A6B-9126-9E24108B56DA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F41" xr:uid="{860860E9-2318-4A6B-9126-9E24108B56DA}">
       <formula1>$F$3:$F$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C12" xr:uid="{8A01CBD2-2D93-4A68-9629-4E4032E64A2C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C36 C40:C41" xr:uid="{8A01CBD2-2D93-4A68-9629-4E4032E64A2C}">
       <formula1>$C$3:$C$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>